<commit_message>
so much **** is corrected it hurts
</commit_message>
<xml_diff>
--- a/Data/Modeling Stage/Feature Selection/R_Gonz_feature_selection_Date_threshold_10.xlsx
+++ b/Data/Modeling Stage/Feature Selection/R_Gonz_feature_selection_Date_threshold_10.xlsx
@@ -47,33 +47,36 @@
     <t>Feature</t>
   </si>
   <si>
+    <t>On/off campus click ratio</t>
+  </si>
+  <si>
+    <t>Total time online (min)</t>
+  </si>
+  <si>
     <t>Number of clicks</t>
   </si>
   <si>
-    <t>On/off campus click ratio</t>
-  </si>
-  <si>
-    <t>Total time online (min)</t>
+    <t>Largest period of inactivity (h)</t>
   </si>
   <si>
     <t>Days with no interaction (%)</t>
   </si>
   <si>
-    <t>Largest period of inactivity (h)</t>
+    <t>Resources viewed</t>
+  </si>
+  <si>
+    <t>Clicks per day</t>
+  </si>
+  <si>
+    <t>Clicks per session</t>
+  </si>
+  <si>
+    <t>Clicks (% of course total)</t>
   </si>
   <si>
     <t>Clicks on course</t>
   </si>
   <si>
-    <t>Clicks per session</t>
-  </si>
-  <si>
-    <t>Clicks (% of course total)</t>
-  </si>
-  <si>
-    <t>Resources viewed</t>
-  </si>
-  <si>
     <t>Start of Session 3 (%)</t>
   </si>
   <si>
@@ -83,10 +86,16 @@
     <t>Start of Session 1 (%)</t>
   </si>
   <si>
+    <t>Average session duration (min)</t>
+  </si>
+  <si>
     <t>Days with no interaction</t>
   </si>
   <si>
-    <t>Average session duration (min)</t>
+    <t>Clicks on campus</t>
+  </si>
+  <si>
+    <t>Average grade of assignments</t>
   </si>
   <si>
     <t>Start of Session 4 (%)</t>
@@ -95,64 +104,55 @@
     <t>Submissions (% of course total)</t>
   </si>
   <si>
-    <t>Clicks per day</t>
-  </si>
-  <si>
-    <t>Clicks on campus</t>
-  </si>
-  <si>
-    <t>Average grade of assignments</t>
+    <t>Assignments viewed</t>
+  </si>
+  <si>
+    <t>Clicks on folder</t>
   </si>
   <si>
     <t>Start of Session 5 (%)</t>
   </si>
   <si>
+    <t>Links viewed</t>
+  </si>
+  <si>
+    <t>Assignments submitted</t>
+  </si>
+  <si>
+    <t>Number of sessions</t>
+  </si>
+  <si>
+    <t>Discussions viewed</t>
+  </si>
+  <si>
+    <t>Quizzes started</t>
+  </si>
+  <si>
     <t>Files downloaded</t>
   </si>
   <si>
+    <t>Clicks on forum</t>
+  </si>
+  <si>
     <t>Number of days</t>
   </si>
   <si>
-    <t>Clicks on folder</t>
-  </si>
-  <si>
-    <t>Assignments viewed</t>
-  </si>
-  <si>
-    <t>Links viewed</t>
-  </si>
-  <si>
-    <t>Discussions viewed</t>
-  </si>
-  <si>
-    <t>Quizzes started</t>
+    <t>Start of Session 10 (%)</t>
+  </si>
+  <si>
+    <t>Start of Session 8 (%)</t>
+  </si>
+  <si>
+    <t>Start of Session 7 (%)</t>
+  </si>
+  <si>
+    <t>Start of Session 6 (%)</t>
   </si>
   <si>
     <t>Forum posts</t>
   </si>
   <si>
-    <t>Assignments submitted</t>
-  </si>
-  <si>
-    <t>Number of sessions</t>
-  </si>
-  <si>
-    <t>Clicks on forum</t>
-  </si>
-  <si>
-    <t>Start of Session 10 (%)</t>
-  </si>
-  <si>
     <t>Start of Session 9 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 8 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 7 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 6 (%)</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -1025,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1033,7 +1033,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1042,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -1057,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1065,10 +1065,10 @@
         <v>26</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1097,16 +1097,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -1161,13 +1161,13 @@
         <v>29</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1225,7 +1225,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1249,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1281,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1292,10 +1292,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1324,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1452,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1516,7 +1516,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -1569,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1747,7 +1747,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1779,16 +1779,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1811,16 +1811,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1875,7 +1875,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -2210,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -2222,18 +2222,18 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -2254,18 +2254,18 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -2274,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -2291,16 +2291,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -2318,18 +2318,18 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -2350,21 +2350,21 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -2382,21 +2382,21 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -2414,21 +2414,21 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -2446,12 +2446,12 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2483,16 +2483,16 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
       <c r="D25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -2515,13 +2515,13 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -2606,12 +2606,12 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>

</xml_diff>